<commit_message>
added Jan 20 month update
</commit_message>
<xml_diff>
--- a/data/ISIMM_2020Jan.xlsx
+++ b/data/ISIMM_2020Jan.xlsx
@@ -13,7 +13,7 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$D$1:$D$626</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$D$1:$D$605</definedName>
     <definedName name="Type_of_location">[1]Dropdown!$C$2:$C$5</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -5686,76 +5686,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>616</xdr:row>
-      <xdr:rowOff>4438</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>617</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000D000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="309562" y="399315298"/>
-          <a:ext cx="68897183" cy="307982"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1800" b="1">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6097,10 +6027,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y626"/>
+  <dimension ref="A1:Y604"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F240" sqref="F240"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -46815,19 +46745,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="626" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H626">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="D1:D626"/>
+  <autoFilter ref="D1:D605"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G221:G315">
       <formula1>Type_of_location</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>